<commit_message>
new submission with unet pc augm score 0.897
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\test submission\codeexecution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4719CDED-99BA-436D-9753-BBFF1240FDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93B7D7-6103-4272-98E5-078F0ECF10CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>['awc', 'qus', 'pxs']</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss</t>
   </si>
 </sst>
 </file>
@@ -376,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +456,7 @@
         <v>0.69299999999999995</v>
       </c>
       <c r="D4">
-        <v>0.72399999999999998</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -471,6 +474,23 @@
       </c>
       <c r="E5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44449</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="D6">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing a new model
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93B7D7-6103-4272-98E5-078F0ECF10CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A4B535-3792-4644-9B1E-F6E97BB5FCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>model_floodwater_unet_pc_augm_diceloss</t>
+  </si>
+  <si>
+    <t>['coz', 'qxb', 'ayt']</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss_2</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_IOUloss</t>
   </si>
 </sst>
 </file>
@@ -379,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +502,34 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44449</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
model with BCE loss, PC and augm
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A4B535-3792-4644-9B1E-F6E97BB5FCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A22CBA-FA6B-4270-9627-4E6E36042190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>model_floodwater_unet_pc_augm_IOUloss</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_BCEloss</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss + model_floodwater_unet_pc_augm_BCEloss</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss + model_floodwater_unet_pc_augm_BCEloss + model_floodwater_unet_pc_augm_IOUloss</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss + model_floodwater_unet_pc_augm_diceloss_2</t>
   </si>
 </sst>
 </file>
@@ -388,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="48.21875" customWidth="1"/>
+    <col min="2" max="2" width="86.21875" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="50.21875" customWidth="1"/>
@@ -530,6 +542,53 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cleaning final model training code
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A22CBA-FA6B-4270-9627-4E6E36042190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93374F87-C3F2-4C84-958C-EB5A96D357B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>model_floodwater_unet_pc_augm_diceloss + model_floodwater_unet_pc_augm_diceloss_2</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss_without_square</t>
+  </si>
+  <si>
+    <t>['hbe', 'jja']</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,6 +595,28 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44456</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
unet pc augm diceloss with 3rd segment of training data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93374F87-C3F2-4C84-958C-EB5A96D357B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE150990-5C6E-4E02-969C-38F973123DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -81,13 +81,31 @@
     <t>model_floodwater_unet_pc_augm_diceloss + model_floodwater_unet_pc_augm_BCEloss + model_floodwater_unet_pc_augm_IOUloss</t>
   </si>
   <si>
-    <t>model_floodwater_unet_pc_augm_diceloss + model_floodwater_unet_pc_augm_diceloss_2</t>
-  </si>
-  <si>
     <t>model_floodwater_unet_pc_augm_diceloss_without_square</t>
   </si>
   <si>
     <t>['hbe', 'jja']</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 3</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss_3</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss_4</t>
+  </si>
+  <si>
+    <t>['pxs', 'tnp'] </t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 3 + 4</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss + 2</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 4</t>
   </si>
 </sst>
 </file>
@@ -406,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,10 +607,13 @@
         <v>44455</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>0.71599999999999997</v>
+      </c>
+      <c r="D12">
+        <v>0.90800000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -600,7 +621,7 @@
         <v>44455</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>0.69799999999999995</v>
@@ -611,10 +632,57 @@
         <v>44456</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>0.68100000000000005</v>
       </c>
       <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model training code commented and clean
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE150990-5C6E-4E02-969C-38F973123DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE01BE27-04BE-44D9-B872-85ECDE773308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 4</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss_5</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 5</t>
+  </si>
+  <si>
+    <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 3 + 4 + 5</t>
   </si>
 </sst>
 </file>
@@ -424,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,6 +693,42 @@
       <c r="B18" t="s">
         <v>26</v>
       </c>
+      <c r="C18">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>0.70399999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>0.71599999999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
preparing submission unet pc augm diceloos 1234
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE01BE27-04BE-44D9-B872-85ECDE773308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB1E511-45B8-4A33-89D6-09F57FB9AE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,7 +622,7 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="D12">
-        <v>0.90800000000000003</v>
+        <v>0.90810000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -659,6 +659,9 @@
       </c>
       <c r="C15">
         <v>0.71799999999999997</v>
+      </c>
+      <c r="D15">
+        <v>0.90869999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
final submission with unet pc augm diceloss 12345
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB1E511-45B8-4A33-89D6-09F57FB9AE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF3280-498C-4D07-AFA7-EB8F457035BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 3 + 4 + 5</t>
+  </si>
+  <si>
+    <t>0.9081</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +681,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44457</v>
       </c>
@@ -689,7 +692,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44459</v>
       </c>
@@ -700,7 +703,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44459</v>
       </c>
@@ -711,7 +714,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44459</v>
       </c>
@@ -721,8 +724,11 @@
       <c r="C20">
         <v>0.71799999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44459</v>
       </c>

</xml_diff>

<commit_message>
updating folder to respect submission format
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlu\Desktop\Machine_Learning\PROJECTS\DRIVENDATA\floodwater_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF3280-498C-4D07-AFA7-EB8F457035BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C065C12A-3B62-452A-BA97-7AEC35577AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>model_floodwater_unet_pc_augm_diceloss 1 +2 + 3 + 4 + 5</t>
-  </si>
-  <si>
-    <t>0.9081</t>
   </si>
 </sst>
 </file>
@@ -438,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -724,8 +721,8 @@
       <c r="C20">
         <v>0.71799999999999997</v>
       </c>
-      <c r="D20" t="s">
-        <v>30</v>
+      <c r="D20">
+        <v>0.90810000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,6 +734,9 @@
       </c>
       <c r="C21">
         <v>0.71599999999999997</v>
+      </c>
+      <c r="D21">
+        <v>0.90820000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>